<commit_message>
OTP, validasi latlng, perbaikan bugs
</commit_message>
<xml_diff>
--- a/input/contoh_excel.xlsx
+++ b/input/contoh_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Project\test Matchain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Project\matchain\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16EA0A4-F9F2-4478-8A13-E2ED17D78FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CB5AB4-06D1-49BD-8534-C50D021587C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>perusahaan_id</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>status_upload</t>
+  </si>
+  <si>
+    <t>kdkab</t>
   </si>
 </sst>
 </file>
@@ -409,50 +412,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>